<commit_message>
Added test for GetGamesFromUser
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Temp/SteamGamesToInstall.xlsx
+++ b/GameGetter/Data/Temp/SteamGamesToInstall.xlsx
@@ -22,19 +22,19 @@
     <x:t>Status</x:t>
   </x:si>
   <x:si>
-    <x:t>Toast Defense</x:t>
+    <x:t>Tiny Toy Tanks</x:t>
   </x:si>
   <x:si>
     <x:t>Received</x:t>
   </x:si>
   <x:si>
-    <x:t>Tiny Toy Tanks</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BatuGame</x:t>
+    <x:t>Super Buckyball Tournament Preseason</x:t>
   </x:si>
   <x:si>
     <x:t>Beat Me! - Puppetonia Tournament</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Perfect Vermin</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>